<commit_message>
Update Variables to include in global and site reports_Curacao_20250321.xlsx
</commit_message>
<xml_diff>
--- a/Variables to include in global and site reports_Curacao_20250321.xlsx
+++ b/Variables to include in global and site reports_Curacao_20250321.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Box\Projects\RMHC on Box\RMHC_Curacao_data_to_global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE99BC4-7481-47C9-A1D3-09BB1688A8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC7283A-63B7-4426-A197-073C78A3F694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37470" yWindow="2220" windowWidth="17505" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4510,8 +4510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E817332-1EA0-456A-B825-F5C8D62F83CA}">
   <dimension ref="A1:E321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="A309" sqref="A309:B309"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6416,7 +6416,7 @@
     </row>
     <row r="165" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A165" s="23" t="s">
-        <v>249</v>
+        <v>836</v>
       </c>
       <c r="B165" s="23" t="s">
         <v>250</v>
@@ -7701,7 +7701,7 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="23" t="s">
-        <v>373</v>
+        <v>1308</v>
       </c>
       <c r="B284" s="23"/>
       <c r="C284" s="23"/>

</xml_diff>